<commit_message>
added statistics values to predict 2017
</commit_message>
<xml_diff>
--- a/Monte_Carlo/HistoricalQuotes_IBM.xlsx
+++ b/Monte_Carlo/HistoricalQuotes_IBM.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IdoYe\PycharmProjects\Industrial_Project_234313\Monte_Carlo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idoye/PycharmProjects/Industrial_Project_234313/Monte_Carlo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{AD4EB1B3-2B7F-489A-8164-AB6EBDB71E27}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D629A2-471C-7F47-9454-C458F812DE84}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12255" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HistoricalQuotes_IBM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1514" uniqueCount="1508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1521" uniqueCount="1509">
   <si>
     <t>drift</t>
   </si>
@@ -4544,6 +4544,9 @@
   </si>
   <si>
     <t>Last 3 Years Statistics</t>
+  </si>
+  <si>
+    <t>2014,2015,2016 Statistics</t>
   </si>
 </sst>
 </file>
@@ -4551,14 +4554,14 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="166" formatCode="[$-1010000]d/m/yyyy;@"/>
-    <numFmt numFmtId="169" formatCode="0.00000000000000000000"/>
+    <numFmt numFmtId="164" formatCode="[$-1010000]d/m/yyyy;@"/>
+    <numFmt numFmtId="165" formatCode="0.00000000000000000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4566,7 +4569,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4574,7 +4577,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Times New Roman"/>
+      <name val="Calibri Light"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="major"/>
@@ -4583,7 +4586,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4592,7 +4595,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4601,7 +4604,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4609,7 +4612,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4617,7 +4620,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4625,7 +4628,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4633,7 +4636,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4642,7 +4645,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4651,7 +4654,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4659,7 +4662,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4668,7 +4671,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4676,7 +4679,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4685,7 +4688,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4694,7 +4697,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4702,7 +4705,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -5054,56 +5057,56 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - הדגשה1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - הדגשה2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - הדגשה3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - הדגשה4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - הדגשה5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - הדגשה6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - הדגשה6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - הדגשה6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="הדגשה1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="הדגשה2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="הדגשה3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="הדגשה4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="הדגשה5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="הדגשה6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="הערה" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="חישוב" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="טוב" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="טקסט אזהרה" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="טקסט הסברי" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="כותרת" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="כותרת 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="כותרת 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="כותרת 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="כותרת 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="ניטראלי" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="סה&quot;כ" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="פלט" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="קלט" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="רע" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="תא מסומן" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="תא מקושר" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5119,7 +5122,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5418,19 +5421,19 @@
   <dimension ref="A1:J2478"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.875" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" style="2" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="20.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1"/>
-    <col min="9" max="9" width="20.375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -5634,6 +5637,12 @@
         <f t="shared" si="0"/>
         <v>-7.0317910863145457E-3</v>
       </c>
+      <c r="F10" s="1" t="s">
+        <v>1508</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>1506</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -5646,6 +5655,13 @@
         <f t="shared" si="0"/>
         <v>1.1889332774442882E-2</v>
       </c>
+      <c r="F11" s="1" t="s">
+        <v>1499</v>
+      </c>
+      <c r="G11" s="3">
+        <f>AVERAGE(C1260:C2015)</f>
+        <v>-1.5110736640663844E-4</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -5658,6 +5674,13 @@
         <f t="shared" si="0"/>
         <v>1.7712704636889381E-3</v>
       </c>
+      <c r="F12" s="1" t="s">
+        <v>1500</v>
+      </c>
+      <c r="G12" s="3">
+        <f>_xlfn.VAR.P(C1260:C2015)</f>
+        <v>1.4805618747182599E-4</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -5670,6 +5693,13 @@
         <f t="shared" si="0"/>
         <v>1.7889983120117792E-2</v>
       </c>
+      <c r="F13" s="1" t="s">
+        <v>1501</v>
+      </c>
+      <c r="G13" s="3">
+        <f>_xlfn.STDEV.P(C1260:C2015)</f>
+        <v>1.2167834132327165E-2</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -5682,6 +5712,13 @@
         <f t="shared" si="0"/>
         <v>4.0205278720898935E-2</v>
       </c>
+      <c r="F14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G14" s="3">
+        <f>G11-(G12/2)</f>
+        <v>-2.2513546014255145E-4</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -5693,6 +5730,13 @@
       <c r="C15" s="1">
         <f t="shared" si="0"/>
         <v>-1.6047025597517445E-2</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
+        <f>B2015</f>
+        <v>166.44</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
update stock values statistics
</commit_message>
<xml_diff>
--- a/Monte_Carlo/HistoricalQuotes_IBM.xlsx
+++ b/Monte_Carlo/HistoricalQuotes_IBM.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idoye/PycharmProjects/Industrial_Project_234313/Monte_Carlo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IdoYe\PycharmProjects\Industrial_Project_234313\Monte_Carlo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D629A2-471C-7F47-9454-C458F812DE84}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{46323D36-E62D-4EE2-9770-0275DB32EA65}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16095" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="HistoricalQuotes_IBM" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -4561,7 +4561,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4569,7 +4569,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4577,7 +4577,7 @@
     <font>
       <sz val="18"/>
       <color theme="3"/>
-      <name val="Calibri Light"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="major"/>
@@ -4586,7 +4586,7 @@
       <b/>
       <sz val="15"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4595,7 +4595,7 @@
       <b/>
       <sz val="13"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4604,7 +4604,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4612,7 +4612,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4620,7 +4620,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4628,7 +4628,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C5700"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4636,7 +4636,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4645,7 +4645,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4654,7 +4654,7 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4662,7 +4662,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4671,7 +4671,7 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4679,7 +4679,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4688,7 +4688,7 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4697,7 +4697,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -4705,7 +4705,7 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
       <scheme val="minor"/>
@@ -5065,48 +5065,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - הדגשה6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - הדגשה6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - הדגשה6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="הדגשה1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="הדגשה2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="הדגשה3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="הדגשה4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="הדגשה5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="הדגשה6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="הערה" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="חישוב" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="טוב" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="טקסט אזהרה" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="טקסט הסברי" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="כותרת" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="כותרת 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="כותרת 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="כותרת 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="כותרת 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="ניטראלי" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="סה&quot;כ" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="פלט" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="קלט" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="רע" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="תא מסומן" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="תא מקושר" xfId="12" builtinId="24" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -5122,7 +5122,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="ערכת נושא Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -5421,19 +5421,19 @@
   <dimension ref="A1:J2478"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.6640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="28.625" style="2" customWidth="1"/>
     <col min="2" max="2" width="13" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="5" width="9" style="1"/>
-    <col min="6" max="6" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.125" style="3" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9" style="1"/>
-    <col min="9" max="9" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
@@ -5482,8 +5482,8 @@
         <v>1499</v>
       </c>
       <c r="J2" s="3">
-        <f>AVERAGE(C1512:C2477)</f>
-        <v>-3.458151651426975E-4</v>
+        <f>AVERAGE(C1764:C2477)</f>
+        <v>-2.247042654684119E-4</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
@@ -5508,8 +5508,8 @@
         <v>1500</v>
       </c>
       <c r="J3" s="3">
-        <f>_xlfn.VAR.P(C1512:C2477)</f>
-        <v>1.4507367819865418E-4</v>
+        <f>_xlfn.VAR.P(C1764:C2477)</f>
+        <v>1.407451506981334E-4</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -5534,8 +5534,8 @@
         <v>1501</v>
       </c>
       <c r="J4" s="3">
-        <f>_xlfn.STDEV.P(C1512:C2477)</f>
-        <v>1.2044653510942279E-2</v>
+        <f>_xlfn.STDEV.P(C1764:C2477)</f>
+        <v>1.1863606142237419E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -5561,7 +5561,7 @@
       </c>
       <c r="J5" s="3">
         <f>J2-(J3/2)</f>
-        <v>-4.1835200424202457E-4</v>
+        <v>-2.950768408174786E-4</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">

</xml_diff>